<commit_message>
Commiting all the data
</commit_message>
<xml_diff>
--- a/DataIN.xlsx
+++ b/DataIN.xlsx
@@ -476,7 +476,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -514,7 +514,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>

</xml_diff>